<commit_message>
Action method are executed!
</commit_message>
<xml_diff>
--- a/scenario/script.xlsx
+++ b/scenario/script.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="script1" sheetId="1" r:id="rId1"/>
@@ -26,17 +26,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="20">
   <si>
     <t>action</t>
   </si>
   <si>
-    <t>input</t>
-  </si>
-  <si>
-    <t>xpath</t>
-  </si>
-  <si>
     <t>description</t>
   </si>
   <si>
@@ -83,6 +77,15 @@
   </si>
   <si>
     <t>//input[@id='txtUsernam']</t>
+  </si>
+  <si>
+    <t>input1</t>
+  </si>
+  <si>
+    <t>input2</t>
+  </si>
+  <si>
+    <t>verifyElementPresent</t>
   </si>
 </sst>
 </file>
@@ -402,90 +405,90 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.42578125" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" customWidth="1"/>
     <col min="3" max="3" width="29" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="D1" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
         <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -497,102 +500,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="22.42578125" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" customWidth="1"/>
-    <col min="3" max="3" width="29" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -605,74 +513,169 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="D1" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
         <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" customWidth="1"/>
+    <col min="3" max="3" width="29" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
         <v>10</v>
       </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>